<commit_message>
updated template, schema and model
</commit_message>
<xml_diff>
--- a/documents/templates/BulkUploadProductionSchedule.xlsx
+++ b/documents/templates/BulkUploadProductionSchedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dineshgajjar/Documents/Work/GitLab/YHWorks/Briot/clients/TMML/server/documents/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF2E197-CCEB-044B-A116-A3BD393E5FCF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{977D4E36-780F-8346-9B53-E1E83C003AFC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="1460" windowWidth="27240" windowHeight="16040" xr2:uid="{6BC27182-73A8-D94B-97E4-67DF06DD5638}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>status</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>Production Schedule Id (of SAP)</t>
+  </si>
+  <si>
+    <t>Scheduled Date</t>
   </si>
 </sst>
 </file>
@@ -413,16 +416,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00918543-CCCC-1A4B-991F-874C25238D88}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="23" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="28" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -437,6 +442,9 @@
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>